<commit_message>
Succeed finding the UT contractor
</commit_message>
<xml_diff>
--- a/Requirement&Actions&Issues&Breakdown.xlsx
+++ b/Requirement&Actions&Issues&Breakdown.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\userdata\q5894c\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MingjingLiu\ForMyself\GitHub\share\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6240" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
   <si>
     <t>ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -956,6 +956,10 @@
   </si>
   <si>
     <t>Raiser</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>已经找到兼职UE设计人员。梁玉婷：微信号：sophieting001</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1558,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1748,12 +1752,15 @@
         <v>43088</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="25.5">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>67</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
add share space project
</commit_message>
<xml_diff>
--- a/Requirement&Actions&Issues&Breakdown.xlsx
+++ b/Requirement&Actions&Issues&Breakdown.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6240" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6240" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="118">
   <si>
     <t>ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -961,6 +961,13 @@
   <si>
     <t>已经找到兼职UE设计人员。梁玉婷：微信号：sophieting001</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>共享空间</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PID0005</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2024,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D6"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2093,6 +2100,14 @@
         <v>103</v>
       </c>
       <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>